<commit_message>
Cambio de color en el texto A y background del X
</commit_message>
<xml_diff>
--- a/sheet/planilla de presentes.xlsx
+++ b/sheet/planilla de presentes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="4" r:id="rId1"/>
@@ -723,7 +723,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM35"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D21" sqref="D21:AH21"/>
     </sheetView>
   </sheetViews>
@@ -2791,7 +2791,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>